<commit_message>
Updated documentation for data comm protocol
</commit_message>
<xml_diff>
--- a/doc/data packet structure.xlsx
+++ b/doc/data packet structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkiselev\Documents\dev\sync_device_32\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73442C3E-6B81-4B87-9FD3-C2587E788801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A57830-4403-430B-A4B5-23BF8D7A1277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{48FB7E95-C391-4754-94A5-34D8116DC883}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{48FB7E95-C391-4754-94A5-34D8116DC883}"/>
   </bookViews>
   <sheets>
     <sheet name="Data packet format" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="115">
   <si>
     <t>Description</t>
   </si>
@@ -771,19 +771,10 @@
     </r>
   </si>
   <si>
-    <t>Setup stroboscopic/ALEX acquisition</t>
-  </si>
-  <si>
     <t>ALX</t>
   </si>
   <si>
     <t>N bursts</t>
-  </si>
-  <si>
-    <t>LSH</t>
-  </si>
-  <si>
-    <t>Enable/disable laser shutters</t>
   </si>
   <si>
     <r>
@@ -799,23 +790,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>enabled</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">(bool) uint32
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>level</t>
     </r>
     <r>
@@ -828,23 +802,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>7</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">(uint8) uint32
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>lasers</t>
     </r>
   </si>
   <si>
@@ -865,34 +822,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">(uint8) uint32
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>lasers</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>15</t>
-    </r>
-  </si>
-  <si>
     <t>15</t>
   </si>
   <si>
@@ -1064,8 +993,111 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Desired time interval between bursts. Values less than </t>
+    <t>TTL level. 0 means low, anything else means high.</t>
+  </si>
+  <si>
+    <t>Timestamp of the first event occurrence, in us. The timestamp is absolute if system timer is stopped, otherwise is relative to current time. A constant delay of 500us is internally added to every timestamp.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Number of event occurences </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. If </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is 0, and interval is given, the event repeats infinitely.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Interval between events, in us. The event repeats </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> times if </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>interval</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is 20+ us, otherwise only once.</t>
+    </r>
+  </si>
+  <si>
+    <t>Commands that set output level (PIN, TGL, PPL, NPL, BST, etc) also configure the given pin as output.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Arduino Due pin name, such as A3 or D51. left-aligned null-terminated string. Refer to </t>
     </r>
     <r>
       <rPr>
@@ -1076,7 +1108,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">(laser exposure + shutter delay + camera readout) x N spectral channels </t>
+      <t>pins.cpp</t>
     </r>
     <r>
       <rPr>
@@ -1086,115 +1118,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>are ignored.</t>
-    </r>
-  </si>
-  <si>
-    <t>TTL level. 0 means low, anything else means high.</t>
-  </si>
-  <si>
-    <t>Timestamp of the first event occurrence, in us. The timestamp is absolute if system timer is stopped, otherwise is relative to current time. A constant delay of 500us is internally added to every timestamp.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Number of event occurences </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>N</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">. If </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>N</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is 0, and interval is given, the event repeats infinitely.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Interval between events, in us. The event repeats </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>N</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> times if </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>interval</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is 20+ us, otherwise only once.</t>
-    </r>
-  </si>
-  <si>
-    <t>Commands that set output level (PIN, TGL, PPL, NPL, BST, etc) also configure the given pin as output.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Arduino Due pin name, such as A3 or D51. left-aligned null-terminated string. Refer to </t>
+      <t xml:space="preserve"> or </t>
     </r>
     <r>
       <rPr>
@@ -1205,7 +1129,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>pins.cpp</t>
+      <t>rev_pin_map.py</t>
     </r>
     <r>
       <rPr>
@@ -1215,7 +1139,30 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> or </t>
+      <t>, as well as Arduino Due pinout diagram.</t>
+    </r>
+  </si>
+  <si>
+    <t>Pulse duration in us. 0 means default duration (100 us).</t>
+  </si>
+  <si>
+    <t>Send a pulse train on TIOA6 pin (aka PC25 or D5) with given pulse period and pulse train duration. It is generated using hardware timer/counter 6 running at 42MHz in waveform mode; the duty cycle is 12.5%. Use this to generate fast bursts of pulses e.g. for reading out camera line-by-line.</t>
+  </si>
+  <si>
+    <t>Enable/disable electrical output of the given pin. If disabled, the pin outputs low TTL level. However, PIN and TGL events still modify the internal level of the disabled pin, which will be visible after the pin is enabled.</t>
+  </si>
+  <si>
+    <t>Start system timer, if is not running. The timer is running by default unless stopped. It always starts with 0.</t>
+  </si>
+  <si>
+    <t>Stopping timer prevents execution of events. The events are scheduled until the timer is active again. Use this to program waveforms with exact timings. Commands STP, CLR, RST also bring all output pins to default low TTL state.</t>
+  </si>
+  <si>
+    <t>Get lookup table for event function names. These functions are identified by their memory address in the event queue.</t>
+  </si>
+  <si>
+    <r>
+      <t>Binary mask indicating what lasers are in use; bit 0 - Cy2, bit 1 - Cy3, bit 2 - Cy5, bit 3 - Cy7. See</t>
     </r>
     <r>
       <rPr>
@@ -1226,7 +1173,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>rev_pin_map.py</t>
+      <t xml:space="preserve"> globals.h</t>
     </r>
     <r>
       <rPr>
@@ -1236,30 +1183,65 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, as well as Arduino Due pinout diagram.</t>
-    </r>
-  </si>
-  <si>
-    <t>Pulse duration in us. 0 means default duration (100 us).</t>
-  </si>
-  <si>
-    <t>Send a pulse train on TIOA6 pin (aka PC25 or D5) with given pulse period and pulse train duration. It is generated using hardware timer/counter 6 running at 42MHz in waveform mode; the duty cycle is 12.5%. Use this to generate fast bursts of pulses e.g. for reading out camera line-by-line.</t>
-  </si>
-  <si>
-    <t>Enable/disable electrical output of the given pin. If disabled, the pin outputs low TTL level. However, PIN and TGL events still modify the internal level of the disabled pin, which will be visible after the pin is enabled.</t>
-  </si>
-  <si>
-    <t>Start system timer, if is not running. The timer is running by default unless stopped. It always starts with 0.</t>
-  </si>
-  <si>
-    <t>Stopping timer prevents execution of events. The events are scheduled until the timer is active again. Use this to program waveforms with exact timings. Commands STP, CLR, RST also bring all output pins to default low TTL state.</t>
-  </si>
-  <si>
-    <t>Get lookup table for event function names. These functions are identified by their memory address in the event queue.</t>
-  </si>
-  <si>
-    <r>
-      <t>Binary mask indicating what lasers are in use; bit 0 - Cy2, bit 1 - Cy3, bit 2 - Cy5, bit 3 - Cy7. See</t>
+      <t xml:space="preserve"> for pin mapping.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">One ASCII line per function in format </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;addr&gt; &lt;name&gt;\n</t>
+    </r>
+  </si>
+  <si>
+    <t>STR</t>
+  </si>
+  <si>
+    <t>Start continious pTIRF
+data acquisition</t>
+  </si>
+  <si>
+    <t>Start stroboscopic pTIRF
+data acquisition</t>
+  </si>
+  <si>
+    <t>Start ALEX pTIRF
+data acquisition</t>
+  </si>
+  <si>
+    <t>CON</t>
+  </si>
+  <si>
+    <t>N frames</t>
+  </si>
+  <si>
+    <r>
+      <t>frame period</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>16</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Desired time interval between bursts/frames. Values less than </t>
     </r>
     <r>
       <rPr>
@@ -1270,7 +1252,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> globals.h</t>
+      <t xml:space="preserve">(laser exposure + shutter delay + camera readout) x N spectral channels </t>
     </r>
     <r>
       <rPr>
@@ -1280,23 +1262,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> for pin mapping.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">One ASCII line per function in format </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;addr&gt; &lt;name&gt;\n</t>
+      <t>are ignored.</t>
     </r>
   </si>
 </sst>
@@ -1473,7 +1439,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1519,30 +1485,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -1557,24 +1499,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1664,65 +1593,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2045,17 +1953,17 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N45"/>
+  <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K45" sqref="A1:K45"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35:K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="1" customWidth="1"/>
+    <col min="3" max="3" width="0.7109375" customWidth="1"/>
     <col min="4" max="4" width="9.140625" customWidth="1"/>
     <col min="5" max="9" width="15" customWidth="1"/>
     <col min="10" max="10" width="0.7109375" customWidth="1"/>
@@ -2065,14 +1973,14 @@
   <sheetData>
     <row r="1" spans="2:13" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="2:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="53" t="s">
+      <c r="D2" s="40" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2163,7 +2071,7 @@
         <v>31</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G6" s="17" t="s">
         <v>11</v>
@@ -2284,10 +2192,10 @@
       <c r="D11" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="19" t="s">
+      <c r="F11" s="41" t="s">
         <v>14</v>
       </c>
       <c r="G11" s="17" t="s">
@@ -2309,10 +2217,10 @@
       <c r="D12" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="19" t="s">
+      <c r="F12" s="41" t="s">
         <v>14</v>
       </c>
       <c r="G12" s="17" t="s">
@@ -2334,13 +2242,21 @@
       <c r="D13" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
+      <c r="E13" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="42" t="s">
+        <v>14</v>
+      </c>
       <c r="J13" s="9"/>
       <c r="K13" s="24"/>
     </row>
@@ -2351,13 +2267,21 @@
       <c r="D14" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
+      <c r="E14" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" s="42" t="s">
+        <v>14</v>
+      </c>
       <c r="J14" s="9"/>
       <c r="K14" s="24"/>
     </row>
@@ -2368,13 +2292,21 @@
       <c r="D15" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
+      <c r="E15" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" s="42" t="s">
+        <v>14</v>
+      </c>
       <c r="J15" s="9"/>
       <c r="K15" s="24"/>
     </row>
@@ -2385,13 +2317,21 @@
       <c r="D16" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
+      <c r="E16" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" s="42" t="s">
+        <v>14</v>
+      </c>
       <c r="J16" s="9"/>
       <c r="K16" s="24"/>
     </row>
@@ -2405,12 +2345,18 @@
       <c r="E17" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="F17" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
+      <c r="F17" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" s="42" t="s">
+        <v>14</v>
+      </c>
       <c r="J17" s="9"/>
       <c r="K17" s="25" t="s">
         <v>60</v>
@@ -2429,11 +2375,15 @@
       <c r="F18" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="G18" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" s="35"/>
-      <c r="I18" s="36"/>
+      <c r="G18" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" s="42" t="s">
+        <v>14</v>
+      </c>
       <c r="J18" s="9"/>
       <c r="K18" s="24"/>
     </row>
@@ -2444,13 +2394,21 @@
       <c r="D19" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
+      <c r="E19" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19" s="42" t="s">
+        <v>14</v>
+      </c>
       <c r="J19" s="9"/>
       <c r="K19" s="25" t="s">
         <v>61</v>
@@ -2463,465 +2421,511 @@
       <c r="D20" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="E20" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
+      <c r="E20" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" s="42" t="s">
+        <v>14</v>
+      </c>
       <c r="J20" s="9"/>
       <c r="K20" s="25" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="40" t="s">
+      <c r="B21" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="45" t="s">
+      <c r="D21" s="36" t="s">
         <v>57</v>
       </c>
       <c r="E21" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="F21" s="46"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="46"/>
-      <c r="I21" s="46"/>
+      <c r="F21" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="42" t="s">
+        <v>14</v>
+      </c>
       <c r="J21" s="9"/>
-      <c r="K21" s="47" t="s">
+      <c r="K21" s="37" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="49" t="s">
-        <v>85</v>
-      </c>
-      <c r="D22" s="41" t="s">
+    <row r="22" spans="1:14" s="33" customFormat="1" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="E22" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="E22" s="42" t="s">
-        <v>90</v>
-      </c>
-      <c r="F22" s="42" t="s">
-        <v>86</v>
-      </c>
-      <c r="G22" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="H22" s="44" t="s">
-        <v>12</v>
-      </c>
-      <c r="I22" s="43" t="s">
-        <v>13</v>
+      <c r="F22" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="I22" s="42" t="s">
+        <v>14</v>
       </c>
       <c r="J22" s="9"/>
       <c r="K22" s="24"/>
-      <c r="M22" t="s">
-        <v>93</v>
+      <c r="M22" s="33" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="48" t="s">
-        <v>81</v>
+      <c r="B23" s="38" t="s">
+        <v>109</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="E23" s="39" t="s">
-        <v>88</v>
-      </c>
-      <c r="F23" s="39" t="s">
-        <v>89</v>
-      </c>
-      <c r="G23" s="17" t="s">
-        <v>11</v>
+        <v>107</v>
+      </c>
+      <c r="E23" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="F23" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="41" t="s">
+        <v>14</v>
       </c>
       <c r="H23" s="18" t="s">
-        <v>83</v>
+        <v>112</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="J23" s="9"/>
       <c r="K23" s="24"/>
-      <c r="M23" s="38" t="s">
+      <c r="M23" s="33" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" s="33" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="E24" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="F24" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="I24" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="J24" s="9"/>
+      <c r="K24" s="24"/>
+      <c r="M24" s="33" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B26" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="1:14" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="43"/>
+      <c r="H27" s="43"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="43"/>
+      <c r="K27" s="43"/>
+    </row>
+    <row r="28" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="43" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
+      <c r="K28" s="43"/>
+    </row>
+    <row r="29" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="43" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="43"/>
+      <c r="J29" s="43"/>
+      <c r="K29" s="43"/>
+    </row>
+    <row r="30" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="43" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" s="43"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="43"/>
+      <c r="J30" s="43"/>
+      <c r="K30" s="43"/>
+    </row>
+    <row r="31" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" s="43"/>
+      <c r="D31" s="43"/>
+      <c r="E31" s="43"/>
+      <c r="F31" s="43"/>
+      <c r="G31" s="43"/>
+      <c r="H31" s="43"/>
+      <c r="I31" s="43"/>
+      <c r="J31" s="43"/>
+      <c r="K31" s="43"/>
+    </row>
+    <row r="32" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" s="43"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="43"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="43"/>
+      <c r="J32" s="43"/>
+      <c r="K32" s="43"/>
+      <c r="N32" s="6"/>
+    </row>
+    <row r="33" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" s="43" t="s">
+        <v>98</v>
+      </c>
+      <c r="C33" s="43"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="43"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="43"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="43"/>
+      <c r="J33" s="43"/>
+      <c r="K33" s="43"/>
+    </row>
+    <row r="34" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="43" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-    </row>
-    <row r="25" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="50" t="s">
-        <v>95</v>
-      </c>
-      <c r="C26" s="50"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="50"/>
-      <c r="G26" s="50"/>
-      <c r="H26" s="50"/>
-      <c r="I26" s="50"/>
-      <c r="J26" s="50"/>
-      <c r="K26" s="50"/>
-    </row>
-    <row r="27" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="B27" s="50" t="s">
-        <v>96</v>
-      </c>
-      <c r="C27" s="50"/>
-      <c r="D27" s="50"/>
-      <c r="E27" s="50"/>
-      <c r="F27" s="50"/>
-      <c r="G27" s="50"/>
-      <c r="H27" s="50"/>
-      <c r="I27" s="50"/>
-      <c r="J27" s="50"/>
-      <c r="K27" s="50"/>
-    </row>
-    <row r="28" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="B28" s="50" t="s">
+      <c r="C34" s="43"/>
+      <c r="D34" s="43"/>
+      <c r="E34" s="43"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="43"/>
+      <c r="H34" s="43"/>
+      <c r="I34" s="43"/>
+      <c r="J34" s="43"/>
+      <c r="K34" s="43"/>
+    </row>
+    <row r="35" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35" s="43"/>
+      <c r="D35" s="43"/>
+      <c r="E35" s="43"/>
+      <c r="F35" s="43"/>
+      <c r="G35" s="43"/>
+      <c r="H35" s="43"/>
+      <c r="I35" s="43"/>
+      <c r="J35" s="43"/>
+      <c r="K35" s="43"/>
+      <c r="N35" s="6"/>
+    </row>
+    <row r="36" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="C36" s="43"/>
+      <c r="D36" s="43"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="43"/>
+      <c r="H36" s="43"/>
+      <c r="I36" s="43"/>
+      <c r="J36" s="43"/>
+      <c r="K36" s="43"/>
+    </row>
+    <row r="37" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="C28" s="50"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="50"/>
-      <c r="G28" s="50"/>
-      <c r="H28" s="50"/>
-      <c r="I28" s="50"/>
-      <c r="J28" s="50"/>
-      <c r="K28" s="50"/>
-    </row>
-    <row r="29" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="52" t="s">
-        <v>17</v>
-      </c>
-      <c r="B29" s="50" t="s">
+      <c r="C37" s="43"/>
+      <c r="D37" s="43"/>
+      <c r="E37" s="43"/>
+      <c r="F37" s="43"/>
+      <c r="G37" s="43"/>
+      <c r="H37" s="43"/>
+      <c r="I37" s="43"/>
+      <c r="J37" s="43"/>
+      <c r="K37" s="43"/>
+    </row>
+    <row r="38" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="50"/>
-      <c r="G29" s="50"/>
-      <c r="H29" s="50"/>
-      <c r="I29" s="50"/>
-      <c r="J29" s="50"/>
-      <c r="K29" s="50"/>
-    </row>
-    <row r="30" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="52" t="s">
-        <v>18</v>
-      </c>
-      <c r="B30" s="50" t="s">
+      <c r="C38" s="43"/>
+      <c r="D38" s="43"/>
+      <c r="E38" s="43"/>
+      <c r="F38" s="43"/>
+      <c r="G38" s="43"/>
+      <c r="H38" s="43"/>
+      <c r="I38" s="43"/>
+      <c r="J38" s="43"/>
+      <c r="K38" s="43"/>
+    </row>
+    <row r="39" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="B39" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="C30" s="50"/>
-      <c r="D30" s="50"/>
-      <c r="E30" s="50"/>
-      <c r="F30" s="50"/>
-      <c r="G30" s="50"/>
-      <c r="H30" s="50"/>
-      <c r="I30" s="50"/>
-      <c r="J30" s="50"/>
-      <c r="K30" s="50"/>
-    </row>
-    <row r="31" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="B31" s="50" t="s">
+      <c r="C39" s="43"/>
+      <c r="D39" s="43"/>
+      <c r="E39" s="43"/>
+      <c r="F39" s="43"/>
+      <c r="G39" s="43"/>
+      <c r="H39" s="43"/>
+      <c r="I39" s="43"/>
+      <c r="J39" s="43"/>
+      <c r="K39" s="43"/>
+    </row>
+    <row r="40" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="B40" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40" s="43"/>
+      <c r="D40" s="43"/>
+      <c r="E40" s="43"/>
+      <c r="F40" s="43"/>
+      <c r="G40" s="43"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="43"/>
+      <c r="J40" s="43"/>
+      <c r="K40" s="43"/>
+    </row>
+    <row r="41" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="B41" s="43" t="s">
         <v>104</v>
       </c>
-      <c r="C31" s="50"/>
-      <c r="D31" s="50"/>
-      <c r="E31" s="50"/>
-      <c r="F31" s="50"/>
-      <c r="G31" s="50"/>
-      <c r="H31" s="50"/>
-      <c r="I31" s="50"/>
-      <c r="J31" s="50"/>
-      <c r="K31" s="50"/>
-      <c r="N31" s="6"/>
-    </row>
-    <row r="32" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="B32" s="50" t="s">
+      <c r="C41" s="43"/>
+      <c r="D41" s="43"/>
+      <c r="E41" s="43"/>
+      <c r="F41" s="43"/>
+      <c r="G41" s="43"/>
+      <c r="H41" s="43"/>
+      <c r="I41" s="43"/>
+      <c r="J41" s="43"/>
+      <c r="K41" s="43"/>
+    </row>
+    <row r="42" spans="1:14" s="33" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" s="45" t="s">
         <v>105</v>
       </c>
-      <c r="C32" s="50"/>
-      <c r="D32" s="50"/>
-      <c r="E32" s="50"/>
-      <c r="F32" s="50"/>
-      <c r="G32" s="50"/>
-      <c r="H32" s="50"/>
-      <c r="I32" s="50"/>
-      <c r="J32" s="50"/>
-      <c r="K32" s="50"/>
-    </row>
-    <row r="33" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="52" t="s">
-        <v>21</v>
-      </c>
-      <c r="B33" s="50" t="s">
-        <v>100</v>
-      </c>
-      <c r="C33" s="50"/>
-      <c r="D33" s="50"/>
-      <c r="E33" s="50"/>
-      <c r="F33" s="50"/>
-      <c r="G33" s="50"/>
-      <c r="H33" s="50"/>
-      <c r="I33" s="50"/>
-      <c r="J33" s="50"/>
-      <c r="K33" s="50"/>
-    </row>
-    <row r="34" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="52" t="s">
-        <v>22</v>
-      </c>
-      <c r="B34" s="50" t="s">
-        <v>106</v>
-      </c>
-      <c r="C34" s="50"/>
-      <c r="D34" s="50"/>
-      <c r="E34" s="50"/>
-      <c r="F34" s="50"/>
-      <c r="G34" s="50"/>
-      <c r="H34" s="50"/>
-      <c r="I34" s="50"/>
-      <c r="J34" s="50"/>
-      <c r="K34" s="50"/>
-      <c r="N34" s="6"/>
-    </row>
-    <row r="35" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="B35" s="50" t="s">
-        <v>107</v>
-      </c>
-      <c r="C35" s="50"/>
-      <c r="D35" s="50"/>
-      <c r="E35" s="50"/>
-      <c r="F35" s="50"/>
-      <c r="G35" s="50"/>
-      <c r="H35" s="50"/>
-      <c r="I35" s="50"/>
-      <c r="J35" s="50"/>
-      <c r="K35" s="50"/>
-    </row>
-    <row r="36" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="52" t="s">
-        <v>24</v>
-      </c>
-      <c r="B36" s="50" t="s">
-        <v>108</v>
-      </c>
-      <c r="C36" s="50"/>
-      <c r="D36" s="50"/>
-      <c r="E36" s="50"/>
-      <c r="F36" s="50"/>
-      <c r="G36" s="50"/>
-      <c r="H36" s="50"/>
-      <c r="I36" s="50"/>
-      <c r="J36" s="50"/>
-      <c r="K36" s="50"/>
-    </row>
-    <row r="37" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="52" t="s">
-        <v>64</v>
-      </c>
-      <c r="B37" s="50" t="s">
-        <v>109</v>
-      </c>
-      <c r="C37" s="50"/>
-      <c r="D37" s="50"/>
-      <c r="E37" s="50"/>
-      <c r="F37" s="50"/>
-      <c r="G37" s="50"/>
-      <c r="H37" s="50"/>
-      <c r="I37" s="50"/>
-      <c r="J37" s="50"/>
-      <c r="K37" s="50"/>
-    </row>
-    <row r="38" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="52" t="s">
-        <v>66</v>
-      </c>
-      <c r="B38" s="50" t="s">
-        <v>110</v>
-      </c>
-      <c r="C38" s="50"/>
-      <c r="D38" s="50"/>
-      <c r="E38" s="50"/>
-      <c r="F38" s="50"/>
-      <c r="G38" s="50"/>
-      <c r="H38" s="50"/>
-      <c r="I38" s="50"/>
-      <c r="J38" s="50"/>
-      <c r="K38" s="50"/>
-    </row>
-    <row r="39" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="52" t="s">
-        <v>68</v>
-      </c>
-      <c r="B39" s="50" t="s">
-        <v>97</v>
-      </c>
-      <c r="C39" s="50"/>
-      <c r="D39" s="50"/>
-      <c r="E39" s="50"/>
-      <c r="F39" s="50"/>
-      <c r="G39" s="50"/>
-      <c r="H39" s="50"/>
-      <c r="I39" s="50"/>
-      <c r="J39" s="50"/>
-      <c r="K39" s="50"/>
-    </row>
-    <row r="40" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="52" t="s">
-        <v>70</v>
-      </c>
-      <c r="B40" s="50" t="s">
-        <v>111</v>
-      </c>
-      <c r="C40" s="50"/>
-      <c r="D40" s="50"/>
-      <c r="E40" s="50"/>
-      <c r="F40" s="50"/>
-      <c r="G40" s="50"/>
-      <c r="H40" s="50"/>
-      <c r="I40" s="50"/>
-      <c r="J40" s="50"/>
-      <c r="K40" s="50"/>
-    </row>
-    <row r="41" spans="1:14" s="38" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="52" t="s">
-        <v>91</v>
-      </c>
-      <c r="B41" s="51" t="s">
-        <v>112</v>
-      </c>
-      <c r="C41" s="51"/>
-      <c r="D41" s="51"/>
-      <c r="E41" s="51"/>
-      <c r="F41" s="51"/>
-      <c r="G41" s="51"/>
-      <c r="H41" s="51"/>
-      <c r="I41" s="51"/>
-      <c r="J41" s="51"/>
-      <c r="K41" s="51"/>
-    </row>
-    <row r="42" spans="1:14" s="38" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="52" t="s">
-        <v>92</v>
-      </c>
-      <c r="B42" s="51" t="s">
-        <v>99</v>
-      </c>
-      <c r="C42" s="51"/>
-      <c r="D42" s="51"/>
-      <c r="E42" s="51"/>
-      <c r="F42" s="51"/>
-      <c r="G42" s="51"/>
-      <c r="H42" s="51"/>
-      <c r="I42" s="51"/>
-      <c r="J42" s="51"/>
-      <c r="K42" s="51"/>
-    </row>
-    <row r="43" spans="1:14" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="37"/>
-      <c r="C43" s="37"/>
-      <c r="D43" s="37"/>
-      <c r="E43" s="37"/>
-      <c r="F43" s="37"/>
-      <c r="G43" s="37"/>
-      <c r="H43" s="37"/>
-      <c r="I43" s="37"/>
-      <c r="J43" s="37"/>
-      <c r="K43" s="37"/>
-    </row>
-    <row r="44" spans="1:14" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="30" t="s">
+      <c r="C42" s="45"/>
+      <c r="D42" s="45"/>
+      <c r="E42" s="45"/>
+      <c r="F42" s="45"/>
+      <c r="G42" s="45"/>
+      <c r="H42" s="45"/>
+      <c r="I42" s="45"/>
+      <c r="J42" s="45"/>
+      <c r="K42" s="45"/>
+    </row>
+    <row r="43" spans="1:14" s="33" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="B43" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="C43" s="45"/>
+      <c r="D43" s="45"/>
+      <c r="E43" s="45"/>
+      <c r="F43" s="45"/>
+      <c r="G43" s="45"/>
+      <c r="H43" s="45"/>
+      <c r="I43" s="45"/>
+      <c r="J43" s="45"/>
+      <c r="K43" s="45"/>
+    </row>
+    <row r="44" spans="1:14" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="44"/>
+      <c r="C44" s="44"/>
+      <c r="D44" s="44"/>
+      <c r="E44" s="44"/>
+      <c r="F44" s="44"/>
+      <c r="G44" s="44"/>
+      <c r="H44" s="44"/>
+      <c r="I44" s="44"/>
+      <c r="J44" s="44"/>
+      <c r="K44" s="44"/>
+    </row>
+    <row r="45" spans="1:14" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="D44" s="29" t="s">
+      <c r="D45" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="E44" s="13" t="s">
+      <c r="E45" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="F44" s="5" t="s">
+      <c r="F45" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G44" s="17" t="s">
+      <c r="G45" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="H44" s="18" t="s">
+      <c r="H45" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="I44" s="17" t="s">
+      <c r="I45" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="J44" s="9"/>
-      <c r="K44" s="31"/>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B45" s="32" t="s">
+      <c r="J45" s="9"/>
+      <c r="K45" s="31"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B46" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="D45">
+      <c r="D46">
         <v>4</v>
       </c>
-      <c r="E45">
+      <c r="E46">
         <v>4</v>
       </c>
-      <c r="F45">
+      <c r="F46">
         <v>4</v>
       </c>
-      <c r="G45">
+      <c r="G46">
         <v>8</v>
       </c>
-      <c r="H45">
+      <c r="H46">
         <v>4</v>
       </c>
-      <c r="I45">
+      <c r="I46">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="E21:I21"/>
+  <mergeCells count="18">
+    <mergeCell ref="B36:K36"/>
+    <mergeCell ref="B44:K44"/>
+    <mergeCell ref="B42:K42"/>
     <mergeCell ref="B43:K43"/>
+    <mergeCell ref="B40:K40"/>
     <mergeCell ref="B41:K41"/>
-    <mergeCell ref="B42:K42"/>
+    <mergeCell ref="B37:K37"/>
+    <mergeCell ref="B38:K38"/>
     <mergeCell ref="B39:K39"/>
-    <mergeCell ref="B40:K40"/>
-    <mergeCell ref="B26:K26"/>
     <mergeCell ref="B27:K27"/>
     <mergeCell ref="B28:K28"/>
     <mergeCell ref="B29:K29"/>
@@ -2931,17 +2935,6 @@
     <mergeCell ref="B33:K33"/>
     <mergeCell ref="B34:K34"/>
     <mergeCell ref="B35:K35"/>
-    <mergeCell ref="B36:K36"/>
-    <mergeCell ref="B37:K37"/>
-    <mergeCell ref="B38:K38"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="E13:I13"/>
-    <mergeCell ref="E14:I14"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="E19:I19"/>
-    <mergeCell ref="E15:I15"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
Added stubs for continuous, strobe, and ALEX acq
</commit_message>
<xml_diff>
--- a/doc/data packet structure.xlsx
+++ b/doc/data packet structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkiselev\Documents\dev\sync_device_32\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A57830-4403-430B-A4B5-23BF8D7A1277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430820CE-E44E-49D6-9EBB-A805CDB8E541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{48FB7E95-C391-4754-94A5-34D8116DC883}"/>
   </bookViews>
@@ -1955,8 +1955,8 @@
   </sheetPr>
   <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35:K35"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2481,8 +2481,8 @@
       <c r="F22" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="G22" s="41" t="s">
-        <v>14</v>
+      <c r="G22" s="17" t="s">
+        <v>11</v>
       </c>
       <c r="H22" s="18" t="s">
         <v>112</v>
@@ -2509,8 +2509,8 @@
       <c r="F23" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="G23" s="41" t="s">
-        <v>14</v>
+      <c r="G23" s="17" t="s">
+        <v>11</v>
       </c>
       <c r="H23" s="18" t="s">
         <v>112</v>
@@ -2537,8 +2537,8 @@
       <c r="F24" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="G24" s="41" t="s">
-        <v>14</v>
+      <c r="G24" s="17" t="s">
+        <v>11</v>
       </c>
       <c r="H24" s="18" t="s">
         <v>82</v>

</xml_diff>

<commit_message>
Updated docs; version number bump to 2.3.0
</commit_message>
<xml_diff>
--- a/doc/data packet structure.xlsx
+++ b/doc/data packet structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkiselev\Documents\dev\sync_device_32\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430820CE-E44E-49D6-9EBB-A805CDB8E541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710E7B59-543D-427F-9983-A0F6ACEBF0E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{48FB7E95-C391-4754-94A5-34D8116DC883}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="114">
   <si>
     <t>Description</t>
   </si>
@@ -828,12 +828,6 @@
     <t>16</t>
   </si>
   <si>
-    <t>Not implemented</t>
-  </si>
-  <si>
-    <t>v2.2.0</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Each data packet is always 24 byte long. A delay of 25+ms between characters resets the data packet.
 On startup, the system prints </t>
@@ -1264,6 +1258,9 @@
       </rPr>
       <t>are ignored.</t>
     </r>
+  </si>
+  <si>
+    <t>v2.3.0</t>
   </si>
 </sst>
 </file>
@@ -1434,7 +1431,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1606,9 +1603,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -1619,6 +1613,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1627,9 +1627,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1955,8 +1952,8 @@
   </sheetPr>
   <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1973,14 +1970,14 @@
   <sheetData>
     <row r="1" spans="2:13" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="2:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="39" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2195,7 +2192,7 @@
       <c r="E11" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="41" t="s">
+      <c r="F11" s="40" t="s">
         <v>14</v>
       </c>
       <c r="G11" s="17" t="s">
@@ -2220,7 +2217,7 @@
       <c r="E12" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="41" t="s">
+      <c r="F12" s="40" t="s">
         <v>14</v>
       </c>
       <c r="G12" s="17" t="s">
@@ -2242,19 +2239,19 @@
       <c r="D13" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" s="42" t="s">
+      <c r="E13" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="41" t="s">
         <v>14</v>
       </c>
       <c r="J13" s="9"/>
@@ -2267,19 +2264,19 @@
       <c r="D14" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14" s="42" t="s">
+      <c r="E14" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" s="41" t="s">
         <v>14</v>
       </c>
       <c r="J14" s="9"/>
@@ -2292,19 +2289,19 @@
       <c r="D15" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="I15" s="42" t="s">
+      <c r="E15" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" s="41" t="s">
         <v>14</v>
       </c>
       <c r="J15" s="9"/>
@@ -2317,19 +2314,19 @@
       <c r="D16" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="G16" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="H16" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="I16" s="42" t="s">
+      <c r="E16" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" s="41" t="s">
         <v>14</v>
       </c>
       <c r="J16" s="9"/>
@@ -2345,16 +2342,16 @@
       <c r="E17" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="F17" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="H17" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="I17" s="42" t="s">
+      <c r="F17" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" s="41" t="s">
         <v>14</v>
       </c>
       <c r="J17" s="9"/>
@@ -2375,13 +2372,13 @@
       <c r="F18" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="G18" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="I18" s="42" t="s">
+      <c r="G18" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" s="41" t="s">
         <v>14</v>
       </c>
       <c r="J18" s="9"/>
@@ -2394,19 +2391,19 @@
       <c r="D19" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="H19" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="I19" s="42" t="s">
+      <c r="E19" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19" s="41" t="s">
         <v>14</v>
       </c>
       <c r="J19" s="9"/>
@@ -2421,24 +2418,24 @@
       <c r="D20" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="E20" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="G20" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="I20" s="42" t="s">
+      <c r="E20" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" s="41" t="s">
         <v>14</v>
       </c>
       <c r="J20" s="9"/>
       <c r="K20" s="25" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2448,19 +2445,19 @@
       <c r="D21" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="E21" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="G21" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="H21" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="I21" s="42" t="s">
+      <c r="E21" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="41" t="s">
         <v>14</v>
       </c>
       <c r="J21" s="9"/>
@@ -2469,64 +2466,59 @@
       </c>
     </row>
     <row r="22" spans="1:14" s="33" customFormat="1" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="38" t="s">
-        <v>108</v>
+      <c r="B22" s="43" t="s">
+        <v>106</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E22" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="F22" s="41" t="s">
+      <c r="F22" s="40" t="s">
         <v>14</v>
       </c>
       <c r="G22" s="17" t="s">
         <v>11</v>
       </c>
       <c r="H22" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="I22" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="I22" s="41" t="s">
         <v>14</v>
       </c>
       <c r="J22" s="9"/>
       <c r="K22" s="24"/>
-      <c r="M22" s="33" t="s">
-        <v>87</v>
-      </c>
     </row>
     <row r="23" spans="1:14" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="38" t="s">
-        <v>109</v>
+      <c r="B23" s="43" t="s">
+        <v>107</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E23" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="F23" s="41" t="s">
+      <c r="F23" s="40" t="s">
         <v>14</v>
       </c>
       <c r="G23" s="17" t="s">
         <v>11</v>
       </c>
       <c r="H23" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J23" s="9"/>
       <c r="K23" s="24"/>
-      <c r="M23" s="33" t="s">
-        <v>87</v>
-      </c>
+      <c r="M23" s="33"/>
     </row>
     <row r="24" spans="1:14" s="33" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="38" t="s">
-        <v>110</v>
+      <c r="B24" s="43" t="s">
+        <v>108</v>
       </c>
       <c r="D24" s="26" t="s">
         <v>81</v>
@@ -2534,7 +2526,7 @@
       <c r="E24" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="F24" s="41" t="s">
+      <c r="F24" s="40" t="s">
         <v>14</v>
       </c>
       <c r="G24" s="17" t="s">
@@ -2544,13 +2536,10 @@
         <v>82</v>
       </c>
       <c r="I24" s="17" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J24" s="9"/>
       <c r="K24" s="24"/>
-      <c r="M24" s="33" t="s">
-        <v>87</v>
-      </c>
     </row>
     <row r="25" spans="1:14" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D25" s="1"/>
@@ -2568,304 +2557,304 @@
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:14" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="43" t="s">
+      <c r="B27" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="44"/>
+      <c r="K27" s="44"/>
+    </row>
+    <row r="28" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="44"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="44"/>
+      <c r="K28" s="44"/>
+    </row>
+    <row r="29" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
+      <c r="K29" s="44"/>
+    </row>
+    <row r="30" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="44" t="s">
+        <v>93</v>
+      </c>
+      <c r="C30" s="44"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="44"/>
+      <c r="J30" s="44"/>
+      <c r="K30" s="44"/>
+    </row>
+    <row r="31" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" s="44"/>
+      <c r="D31" s="44"/>
+      <c r="E31" s="44"/>
+      <c r="F31" s="44"/>
+      <c r="G31" s="44"/>
+      <c r="H31" s="44"/>
+      <c r="I31" s="44"/>
+      <c r="J31" s="44"/>
+      <c r="K31" s="44"/>
+    </row>
+    <row r="32" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="44" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32" s="44"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="44"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="44"/>
+      <c r="I32" s="44"/>
+      <c r="J32" s="44"/>
+      <c r="K32" s="44"/>
+      <c r="N32" s="6"/>
+    </row>
+    <row r="33" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" s="44" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" s="44"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="44"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="44"/>
+      <c r="I33" s="44"/>
+      <c r="J33" s="44"/>
+      <c r="K33" s="44"/>
+    </row>
+    <row r="34" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="44" t="s">
+        <v>91</v>
+      </c>
+      <c r="C34" s="44"/>
+      <c r="D34" s="44"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="44"/>
+      <c r="G34" s="44"/>
+      <c r="H34" s="44"/>
+      <c r="I34" s="44"/>
+      <c r="J34" s="44"/>
+      <c r="K34" s="44"/>
+    </row>
+    <row r="35" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="C35" s="44"/>
+      <c r="D35" s="44"/>
+      <c r="E35" s="44"/>
+      <c r="F35" s="44"/>
+      <c r="G35" s="44"/>
+      <c r="H35" s="44"/>
+      <c r="I35" s="44"/>
+      <c r="J35" s="44"/>
+      <c r="K35" s="44"/>
+      <c r="N35" s="6"/>
+    </row>
+    <row r="36" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" s="44" t="s">
+        <v>98</v>
+      </c>
+      <c r="C36" s="44"/>
+      <c r="D36" s="44"/>
+      <c r="E36" s="44"/>
+      <c r="F36" s="44"/>
+      <c r="G36" s="44"/>
+      <c r="H36" s="44"/>
+      <c r="I36" s="44"/>
+      <c r="J36" s="44"/>
+      <c r="K36" s="44"/>
+    </row>
+    <row r="37" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" s="44" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" s="44"/>
+      <c r="D37" s="44"/>
+      <c r="E37" s="44"/>
+      <c r="F37" s="44"/>
+      <c r="G37" s="44"/>
+      <c r="H37" s="44"/>
+      <c r="I37" s="44"/>
+      <c r="J37" s="44"/>
+      <c r="K37" s="44"/>
+    </row>
+    <row r="38" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" s="44" t="s">
+        <v>100</v>
+      </c>
+      <c r="C38" s="44"/>
+      <c r="D38" s="44"/>
+      <c r="E38" s="44"/>
+      <c r="F38" s="44"/>
+      <c r="G38" s="44"/>
+      <c r="H38" s="44"/>
+      <c r="I38" s="44"/>
+      <c r="J38" s="44"/>
+      <c r="K38" s="44"/>
+    </row>
+    <row r="39" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="B39" s="44" t="s">
+        <v>101</v>
+      </c>
+      <c r="C39" s="44"/>
+      <c r="D39" s="44"/>
+      <c r="E39" s="44"/>
+      <c r="F39" s="44"/>
+      <c r="G39" s="44"/>
+      <c r="H39" s="44"/>
+      <c r="I39" s="44"/>
+      <c r="J39" s="44"/>
+      <c r="K39" s="44"/>
+    </row>
+    <row r="40" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="B40" s="44" t="s">
         <v>89</v>
       </c>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="43"/>
-      <c r="H27" s="43"/>
-      <c r="I27" s="43"/>
-      <c r="J27" s="43"/>
-      <c r="K27" s="43"/>
-    </row>
-    <row r="28" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="B28" s="43" t="s">
-        <v>90</v>
-      </c>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
-      <c r="K28" s="43"/>
-    </row>
-    <row r="29" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="39" t="s">
-        <v>16</v>
-      </c>
-      <c r="B29" s="43" t="s">
-        <v>94</v>
-      </c>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="43"/>
-      <c r="K29" s="43"/>
-    </row>
-    <row r="30" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="B30" s="43" t="s">
-        <v>95</v>
-      </c>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="43"/>
-      <c r="I30" s="43"/>
-      <c r="J30" s="43"/>
-      <c r="K30" s="43"/>
-    </row>
-    <row r="31" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="B31" s="43" t="s">
-        <v>96</v>
-      </c>
-      <c r="C31" s="43"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="43"/>
-      <c r="H31" s="43"/>
-      <c r="I31" s="43"/>
-      <c r="J31" s="43"/>
-      <c r="K31" s="43"/>
-    </row>
-    <row r="32" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="B32" s="43" t="s">
-        <v>97</v>
-      </c>
-      <c r="C32" s="43"/>
-      <c r="D32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="F32" s="43"/>
-      <c r="G32" s="43"/>
-      <c r="H32" s="43"/>
-      <c r="I32" s="43"/>
-      <c r="J32" s="43"/>
-      <c r="K32" s="43"/>
-      <c r="N32" s="6"/>
-    </row>
-    <row r="33" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="B33" s="43" t="s">
-        <v>98</v>
-      </c>
-      <c r="C33" s="43"/>
-      <c r="D33" s="43"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="43"/>
-      <c r="G33" s="43"/>
-      <c r="H33" s="43"/>
-      <c r="I33" s="43"/>
-      <c r="J33" s="43"/>
-      <c r="K33" s="43"/>
-    </row>
-    <row r="34" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="B34" s="43" t="s">
-        <v>93</v>
-      </c>
-      <c r="C34" s="43"/>
-      <c r="D34" s="43"/>
-      <c r="E34" s="43"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="43"/>
-      <c r="H34" s="43"/>
-      <c r="I34" s="43"/>
-      <c r="J34" s="43"/>
-      <c r="K34" s="43"/>
-    </row>
-    <row r="35" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="B35" s="43" t="s">
-        <v>99</v>
-      </c>
-      <c r="C35" s="43"/>
-      <c r="D35" s="43"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="43"/>
-      <c r="H35" s="43"/>
-      <c r="I35" s="43"/>
-      <c r="J35" s="43"/>
-      <c r="K35" s="43"/>
-      <c r="N35" s="6"/>
-    </row>
-    <row r="36" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="B36" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="C36" s="43"/>
-      <c r="D36" s="43"/>
-      <c r="E36" s="43"/>
-      <c r="F36" s="43"/>
-      <c r="G36" s="43"/>
-      <c r="H36" s="43"/>
-      <c r="I36" s="43"/>
-      <c r="J36" s="43"/>
-      <c r="K36" s="43"/>
-    </row>
-    <row r="37" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="39" t="s">
-        <v>24</v>
-      </c>
-      <c r="B37" s="43" t="s">
-        <v>101</v>
-      </c>
-      <c r="C37" s="43"/>
-      <c r="D37" s="43"/>
-      <c r="E37" s="43"/>
-      <c r="F37" s="43"/>
-      <c r="G37" s="43"/>
-      <c r="H37" s="43"/>
-      <c r="I37" s="43"/>
-      <c r="J37" s="43"/>
-      <c r="K37" s="43"/>
-    </row>
-    <row r="38" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="39" t="s">
-        <v>64</v>
-      </c>
-      <c r="B38" s="43" t="s">
+      <c r="C40" s="44"/>
+      <c r="D40" s="44"/>
+      <c r="E40" s="44"/>
+      <c r="F40" s="44"/>
+      <c r="G40" s="44"/>
+      <c r="H40" s="44"/>
+      <c r="I40" s="44"/>
+      <c r="J40" s="44"/>
+      <c r="K40" s="44"/>
+    </row>
+    <row r="41" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="B41" s="44" t="s">
         <v>102</v>
       </c>
-      <c r="C38" s="43"/>
-      <c r="D38" s="43"/>
-      <c r="E38" s="43"/>
-      <c r="F38" s="43"/>
-      <c r="G38" s="43"/>
-      <c r="H38" s="43"/>
-      <c r="I38" s="43"/>
-      <c r="J38" s="43"/>
-      <c r="K38" s="43"/>
-    </row>
-    <row r="39" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="B39" s="43" t="s">
+      <c r="C41" s="44"/>
+      <c r="D41" s="44"/>
+      <c r="E41" s="44"/>
+      <c r="F41" s="44"/>
+      <c r="G41" s="44"/>
+      <c r="H41" s="44"/>
+      <c r="I41" s="44"/>
+      <c r="J41" s="44"/>
+      <c r="K41" s="44"/>
+    </row>
+    <row r="42" spans="1:14" s="33" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" s="46" t="s">
         <v>103</v>
       </c>
-      <c r="C39" s="43"/>
-      <c r="D39" s="43"/>
-      <c r="E39" s="43"/>
-      <c r="F39" s="43"/>
-      <c r="G39" s="43"/>
-      <c r="H39" s="43"/>
-      <c r="I39" s="43"/>
-      <c r="J39" s="43"/>
-      <c r="K39" s="43"/>
-    </row>
-    <row r="40" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="B40" s="43" t="s">
-        <v>91</v>
-      </c>
-      <c r="C40" s="43"/>
-      <c r="D40" s="43"/>
-      <c r="E40" s="43"/>
-      <c r="F40" s="43"/>
-      <c r="G40" s="43"/>
-      <c r="H40" s="43"/>
-      <c r="I40" s="43"/>
-      <c r="J40" s="43"/>
-      <c r="K40" s="43"/>
-    </row>
-    <row r="41" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="39" t="s">
-        <v>70</v>
-      </c>
-      <c r="B41" s="43" t="s">
-        <v>104</v>
-      </c>
-      <c r="C41" s="43"/>
-      <c r="D41" s="43"/>
-      <c r="E41" s="43"/>
-      <c r="F41" s="43"/>
-      <c r="G41" s="43"/>
-      <c r="H41" s="43"/>
-      <c r="I41" s="43"/>
-      <c r="J41" s="43"/>
-      <c r="K41" s="43"/>
-    </row>
-    <row r="42" spans="1:14" s="33" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="39" t="s">
-        <v>85</v>
-      </c>
-      <c r="B42" s="45" t="s">
-        <v>105</v>
-      </c>
-      <c r="C42" s="45"/>
-      <c r="D42" s="45"/>
-      <c r="E42" s="45"/>
-      <c r="F42" s="45"/>
-      <c r="G42" s="45"/>
-      <c r="H42" s="45"/>
-      <c r="I42" s="45"/>
-      <c r="J42" s="45"/>
-      <c r="K42" s="45"/>
+      <c r="C42" s="46"/>
+      <c r="D42" s="46"/>
+      <c r="E42" s="46"/>
+      <c r="F42" s="46"/>
+      <c r="G42" s="46"/>
+      <c r="H42" s="46"/>
+      <c r="I42" s="46"/>
+      <c r="J42" s="46"/>
+      <c r="K42" s="46"/>
     </row>
     <row r="43" spans="1:14" s="33" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="39" t="s">
+      <c r="A43" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="B43" s="45" t="s">
-        <v>114</v>
-      </c>
-      <c r="C43" s="45"/>
-      <c r="D43" s="45"/>
-      <c r="E43" s="45"/>
-      <c r="F43" s="45"/>
-      <c r="G43" s="45"/>
-      <c r="H43" s="45"/>
-      <c r="I43" s="45"/>
-      <c r="J43" s="45"/>
-      <c r="K43" s="45"/>
+      <c r="B43" s="46" t="s">
+        <v>112</v>
+      </c>
+      <c r="C43" s="46"/>
+      <c r="D43" s="46"/>
+      <c r="E43" s="46"/>
+      <c r="F43" s="46"/>
+      <c r="G43" s="46"/>
+      <c r="H43" s="46"/>
+      <c r="I43" s="46"/>
+      <c r="J43" s="46"/>
+      <c r="K43" s="46"/>
     </row>
     <row r="44" spans="1:14" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="44"/>
-      <c r="C44" s="44"/>
-      <c r="D44" s="44"/>
-      <c r="E44" s="44"/>
-      <c r="F44" s="44"/>
-      <c r="G44" s="44"/>
-      <c r="H44" s="44"/>
-      <c r="I44" s="44"/>
-      <c r="J44" s="44"/>
-      <c r="K44" s="44"/>
+      <c r="B44" s="45"/>
+      <c r="C44" s="45"/>
+      <c r="D44" s="45"/>
+      <c r="E44" s="45"/>
+      <c r="F44" s="45"/>
+      <c r="G44" s="45"/>
+      <c r="H44" s="45"/>
+      <c r="I44" s="45"/>
+      <c r="J44" s="45"/>
+      <c r="K44" s="45"/>
     </row>
     <row r="45" spans="1:14" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="30" t="s">
@@ -2917,6 +2906,15 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B32:K32"/>
+    <mergeCell ref="B33:K33"/>
+    <mergeCell ref="B34:K34"/>
+    <mergeCell ref="B35:K35"/>
+    <mergeCell ref="B27:K27"/>
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B29:K29"/>
+    <mergeCell ref="B30:K30"/>
+    <mergeCell ref="B31:K31"/>
     <mergeCell ref="B36:K36"/>
     <mergeCell ref="B44:K44"/>
     <mergeCell ref="B42:K42"/>
@@ -2926,15 +2924,6 @@
     <mergeCell ref="B37:K37"/>
     <mergeCell ref="B38:K38"/>
     <mergeCell ref="B39:K39"/>
-    <mergeCell ref="B27:K27"/>
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B29:K29"/>
-    <mergeCell ref="B30:K30"/>
-    <mergeCell ref="B31:K31"/>
-    <mergeCell ref="B32:K32"/>
-    <mergeCell ref="B33:K33"/>
-    <mergeCell ref="B34:K34"/>
-    <mergeCell ref="B35:K35"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
docs: fixed minor errors in data packet structure document
</commit_message>
<xml_diff>
--- a/doc/data packet structure.xlsx
+++ b/doc/data packet structure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkiselev\Documents\dev\sync_device_32\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkiselev\Documents\dev\microsync\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{284D98A1-A11C-46F5-BB4C-BDF0125C09D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E723593C-D3C0-460F-AA35-0B0B832B6477}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{48FB7E95-C391-4754-94A5-34D8116DC883}"/>
+    <workbookView xWindow="8700" yWindow="1710" windowWidth="40620" windowHeight="17700" xr2:uid="{48FB7E95-C391-4754-94A5-34D8116DC883}"/>
   </bookViews>
   <sheets>
     <sheet name="Data packet format" sheetId="2" r:id="rId1"/>
@@ -829,6 +829,389 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cmd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> field is 4-character long, left-aligned. That is, for 3-character commands, the last byte is ignored. The commands are case-insensitive. Unknown command leads to error response.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">See </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SysProps</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> enum for a list of supported properties. Property names start with </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ro_ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">or </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rw_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (read-only or read-write).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>burst period</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>16</t>
+    </r>
+  </si>
+  <si>
+    <t>TTL level. 0 means low, anything else means high.</t>
+  </si>
+  <si>
+    <t>Timestamp of the first event occurrence, in us. The timestamp is absolute if system timer is stopped, otherwise is relative to current time. A constant delay of 500us is internally added to every timestamp.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Number of event occurences </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. If </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is 0, and interval is given, the event repeats infinitely.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Interval between events, in us. The event repeats </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> times if </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>interval</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is 20+ us, otherwise only once.</t>
+    </r>
+  </si>
+  <si>
+    <t>Commands that set output level (PIN, TGL, PPL, NPL, BST, etc) also configure the given pin as output.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Arduino Due pin name, such as A3 or D51. left-aligned null-terminated string. Refer to </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pins.cpp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rev_pin_map.py</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, as well as Arduino Due pinout diagram.</t>
+    </r>
+  </si>
+  <si>
+    <t>Pulse duration in us. 0 means default duration (100 us).</t>
+  </si>
+  <si>
+    <t>Send a pulse train on TIOA6 pin (aka PC25 or D5) with given pulse period and pulse train duration. It is generated using hardware timer/counter 6 running at 42MHz in waveform mode; the duty cycle is 12.5%. Use this to generate fast bursts of pulses e.g. for reading out camera line-by-line.</t>
+  </si>
+  <si>
+    <t>Enable/disable electrical output of the given pin. If disabled, the pin outputs low TTL level. However, PIN and TGL events still modify the internal level of the disabled pin, which will be visible after the pin is enabled.</t>
+  </si>
+  <si>
+    <t>Start system timer, if is not running. The timer is running by default unless stopped. It always starts with 0.</t>
+  </si>
+  <si>
+    <t>Stopping timer prevents execution of events. The events are scheduled until the timer is active again. Use this to program waveforms with exact timings. Commands STP, CLR, RST also bring all output pins to default low TTL state.</t>
+  </si>
+  <si>
+    <t>Get lookup table for event function names. These functions are identified by their memory address in the event queue.</t>
+  </si>
+  <si>
+    <r>
+      <t>Binary mask indicating what lasers are in use; bit 0 - Cy2, bit 1 - Cy3, bit 2 - Cy5, bit 3 - Cy7. See</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> globals.h</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for pin mapping.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">One ASCII line per function in format </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;addr&gt; &lt;name&gt;\n</t>
+    </r>
+  </si>
+  <si>
+    <t>STR</t>
+  </si>
+  <si>
+    <t>Start continious pTIRF
+data acquisition</t>
+  </si>
+  <si>
+    <t>Start stroboscopic pTIRF
+data acquisition</t>
+  </si>
+  <si>
+    <t>Start ALEX pTIRF
+data acquisition</t>
+  </si>
+  <si>
+    <t>CON</t>
+  </si>
+  <si>
+    <t>N frames</t>
+  </si>
+  <si>
+    <r>
+      <t>frame period</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>16</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Desired time interval between bursts/frames. Values less than </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(laser exposure + shutter delay + camera readout) x N spectral channels </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>are ignored.</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">Each data packet is always 24 byte long. A delay of 25+ms between characters resets the data packet.
 On startup, the system prints </t>
     </r>
@@ -852,7 +1235,7 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-In case of errors, the replay is </t>
+In case of errors, the reply is </t>
     </r>
     <r>
       <rPr>
@@ -877,390 +1260,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">The </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>cmd</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> field is 4-character long, left-aligned. That is, for 3-character commands, the last byte is ignored. The commands are case-insensitive. Unknown command leads to error response.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">See </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>SysProps</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> enum for a list of supported properties. Property names start with </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">ro_ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">or </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>rw_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (read-only or read-write).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>burst period</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>16</t>
-    </r>
-  </si>
-  <si>
-    <t>TTL level. 0 means low, anything else means high.</t>
-  </si>
-  <si>
-    <t>Timestamp of the first event occurrence, in us. The timestamp is absolute if system timer is stopped, otherwise is relative to current time. A constant delay of 500us is internally added to every timestamp.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Number of event occurences </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>N</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">. If </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>N</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is 0, and interval is given, the event repeats infinitely.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Interval between events, in us. The event repeats </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>N</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> times if </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>interval</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is 20+ us, otherwise only once.</t>
-    </r>
-  </si>
-  <si>
-    <t>Commands that set output level (PIN, TGL, PPL, NPL, BST, etc) also configure the given pin as output.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Arduino Due pin name, such as A3 or D51. left-aligned null-terminated string. Refer to </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>pins.cpp</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> or </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>rev_pin_map.py</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, as well as Arduino Due pinout diagram.</t>
-    </r>
-  </si>
-  <si>
-    <t>Pulse duration in us. 0 means default duration (100 us).</t>
-  </si>
-  <si>
-    <t>Send a pulse train on TIOA6 pin (aka PC25 or D5) with given pulse period and pulse train duration. It is generated using hardware timer/counter 6 running at 42MHz in waveform mode; the duty cycle is 12.5%. Use this to generate fast bursts of pulses e.g. for reading out camera line-by-line.</t>
-  </si>
-  <si>
-    <t>Enable/disable electrical output of the given pin. If disabled, the pin outputs low TTL level. However, PIN and TGL events still modify the internal level of the disabled pin, which will be visible after the pin is enabled.</t>
-  </si>
-  <si>
-    <t>Start system timer, if is not running. The timer is running by default unless stopped. It always starts with 0.</t>
-  </si>
-  <si>
-    <t>Stopping timer prevents execution of events. The events are scheduled until the timer is active again. Use this to program waveforms with exact timings. Commands STP, CLR, RST also bring all output pins to default low TTL state.</t>
-  </si>
-  <si>
-    <t>Get lookup table for event function names. These functions are identified by their memory address in the event queue.</t>
-  </si>
-  <si>
-    <r>
-      <t>Binary mask indicating what lasers are in use; bit 0 - Cy2, bit 1 - Cy3, bit 2 - Cy5, bit 3 - Cy7. See</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> globals.h</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> for pin mapping.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">One ASCII line per function in format </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;addr&gt; &lt;name&gt;\n</t>
-    </r>
-  </si>
-  <si>
-    <t>STR</t>
-  </si>
-  <si>
-    <t>Start continious pTIRF
-data acquisition</t>
-  </si>
-  <si>
-    <t>Start stroboscopic pTIRF
-data acquisition</t>
-  </si>
-  <si>
-    <t>Start ALEX pTIRF
-data acquisition</t>
-  </si>
-  <si>
-    <t>CON</t>
-  </si>
-  <si>
-    <t>N frames</t>
-  </si>
-  <si>
-    <r>
-      <t>frame period</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>16</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Desired time interval between bursts/frames. Values less than </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">(laser exposure + shutter delay + camera readout) x N spectral channels </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>are ignored.</t>
-    </r>
-  </si>
-  <si>
-    <t>v2.3.0</t>
+    <t>v2.4.0</t>
   </si>
 </sst>
 </file>
@@ -1500,7 +1500,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1517,16 +1517,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1551,16 +1550,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1578,35 +1568,27 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1660,9 +1642,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1700,7 +1682,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1806,7 +1788,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1948,7 +1930,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1961,8 +1943,8 @@
   </sheetPr>
   <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1973,7 +1955,7 @@
     <col min="4" max="4" width="9.140625" customWidth="1"/>
     <col min="5" max="9" width="15" customWidth="1"/>
     <col min="10" max="10" width="0.7109375" customWidth="1"/>
-    <col min="11" max="11" width="31.28515625" style="11" customWidth="1"/>
+    <col min="11" max="11" width="31.28515625" customWidth="1"/>
     <col min="13" max="13" width="38.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1986,7 +1968,7 @@
       </c>
     </row>
     <row r="2" spans="2:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="39" t="s">
+      <c r="D2" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1994,22 +1976,22 @@
       <c r="B3" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="1">
         <v>0</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E3" s="1">
         <v>1</v>
       </c>
-      <c r="F3" s="21">
+      <c r="F3" s="1">
         <v>2</v>
       </c>
-      <c r="G3" s="21">
+      <c r="G3" s="1">
         <v>3</v>
       </c>
-      <c r="H3" s="21">
+      <c r="H3" s="1">
         <v>4</v>
       </c>
-      <c r="I3" s="21">
+      <c r="I3" s="1">
         <v>5</v>
       </c>
     </row>
@@ -2017,60 +1999,60 @@
       <c r="B4" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="1">
         <v>4</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="1">
         <v>4</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="1">
         <v>4</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="1">
         <v>4</v>
       </c>
-      <c r="H4" s="21">
+      <c r="H4" s="1">
         <v>4</v>
       </c>
-      <c r="I4" s="21">
+      <c r="I4" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="2:13" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="11" t="s">
         <v>29</v>
       </c>
       <c r="J5" s="8"/>
-      <c r="K5" s="23" t="s">
+      <c r="K5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="L5" s="22"/>
-      <c r="M5" s="22"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
     </row>
     <row r="6" spans="2:13" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="5" t="s">
@@ -2079,48 +2061,48 @@
       <c r="F6" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="H6" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="I6" s="16" t="s">
         <v>13</v>
       </c>
       <c r="J6" s="9"/>
-      <c r="K6" s="24"/>
+      <c r="K6" s="20"/>
     </row>
     <row r="7" spans="2:13" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="23" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="17" t="s">
+      <c r="F7" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="17" t="s">
+      <c r="I7" s="16" t="s">
         <v>13</v>
       </c>
       <c r="J7" s="10"/>
-      <c r="K7" s="24"/>
+      <c r="K7" s="20"/>
     </row>
     <row r="8" spans="2:13" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="5" t="s">
@@ -2129,23 +2111,23 @@
       <c r="F8" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="17" t="s">
+      <c r="H8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="17" t="s">
+      <c r="I8" s="16" t="s">
         <v>13</v>
       </c>
       <c r="J8" s="9"/>
-      <c r="K8" s="24"/>
+      <c r="K8" s="20"/>
     </row>
     <row r="9" spans="2:13" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="22" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="5" t="s">
@@ -2154,401 +2136,400 @@
       <c r="F9" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="17" t="s">
+      <c r="H9" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="17" t="s">
+      <c r="I9" s="16" t="s">
         <v>13</v>
       </c>
       <c r="J9" s="9"/>
-      <c r="K9" s="24"/>
+      <c r="K9" s="20"/>
     </row>
     <row r="10" spans="2:13" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="12" t="s">
         <v>34</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="G10" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="H10" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="17" t="s">
+      <c r="I10" s="16" t="s">
         <v>13</v>
       </c>
       <c r="J10" s="10"/>
-      <c r="K10" s="24"/>
+      <c r="K10" s="20"/>
     </row>
     <row r="11" spans="2:13" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="E11" s="34" t="s">
+      <c r="E11" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="17" t="s">
+      <c r="F11" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="18" t="s">
+      <c r="H11" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="17" t="s">
+      <c r="I11" s="16" t="s">
         <v>13</v>
       </c>
       <c r="J11" s="10"/>
-      <c r="K11" s="24"/>
+      <c r="K11" s="20"/>
     </row>
     <row r="12" spans="2:13" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="D12" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="E12" s="34" t="s">
+      <c r="E12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" s="17" t="s">
+      <c r="F12" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="18" t="s">
+      <c r="H12" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="17" t="s">
+      <c r="I12" s="16" t="s">
         <v>13</v>
       </c>
       <c r="J12" s="10"/>
-      <c r="K12" s="24"/>
+      <c r="K12" s="20"/>
     </row>
     <row r="13" spans="2:13" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="26" t="s">
+      <c r="D13" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" s="40" t="s">
+      <c r="E13" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="32" t="s">
         <v>14</v>
       </c>
       <c r="J13" s="9"/>
-      <c r="K13" s="24"/>
+      <c r="K13" s="20"/>
     </row>
     <row r="14" spans="2:13" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="26" t="s">
+      <c r="D14" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14" s="40" t="s">
+      <c r="E14" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" s="32" t="s">
         <v>14</v>
       </c>
       <c r="J14" s="9"/>
-      <c r="K14" s="24"/>
+      <c r="K14" s="20"/>
     </row>
     <row r="15" spans="2:13" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="26" t="s">
+      <c r="D15" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="I15" s="40" t="s">
+      <c r="E15" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" s="32" t="s">
         <v>14</v>
       </c>
       <c r="J15" s="9"/>
-      <c r="K15" s="24"/>
+      <c r="K15" s="20"/>
     </row>
     <row r="16" spans="2:13" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D16" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="G16" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="H16" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="I16" s="40" t="s">
+      <c r="E16" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" s="32" t="s">
         <v>14</v>
       </c>
       <c r="J16" s="9"/>
-      <c r="K16" s="24"/>
+      <c r="K16" s="20"/>
     </row>
     <row r="17" spans="1:14" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="26" t="s">
+      <c r="D17" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="F17" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="H17" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="I17" s="40" t="s">
+      <c r="F17" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" s="32" t="s">
         <v>14</v>
       </c>
       <c r="J17" s="9"/>
-      <c r="K17" s="25" t="s">
+      <c r="K17" s="21" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="D18" s="26" t="s">
+      <c r="D18" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="E18" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F18" s="13" t="s">
+      <c r="F18" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="G18" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="I18" s="40" t="s">
+      <c r="G18" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" s="32" t="s">
         <v>14</v>
       </c>
       <c r="J18" s="9"/>
-      <c r="K18" s="24"/>
+      <c r="K18" s="20"/>
     </row>
     <row r="19" spans="1:14" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="26" t="s">
+      <c r="D19" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="H19" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="I19" s="40" t="s">
+      <c r="E19" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19" s="32" t="s">
         <v>14</v>
       </c>
       <c r="J19" s="9"/>
-      <c r="K19" s="25" t="s">
+      <c r="K19" s="21" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="D20" s="26" t="s">
+      <c r="D20" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="E20" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="G20" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="I20" s="40" t="s">
+      <c r="E20" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" s="32" t="s">
         <v>14</v>
       </c>
       <c r="J20" s="9"/>
-      <c r="K20" s="25" t="s">
+      <c r="K20" s="21" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="J21" s="9"/>
+      <c r="K21" s="30" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="F22" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="I22" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" s="9"/>
+      <c r="K22" s="20"/>
+    </row>
+    <row r="23" spans="1:14" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="D23" s="22" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="E21" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="G21" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="H21" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="I21" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="J21" s="9"/>
-      <c r="K21" s="37" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" s="33" customFormat="1" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="41" t="s">
-        <v>106</v>
-      </c>
-      <c r="D22" s="26" t="s">
+      <c r="E23" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F23" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="E22" s="42" t="s">
+      <c r="I23" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="J23" s="9"/>
+      <c r="K23" s="20"/>
+    </row>
+    <row r="24" spans="1:14" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F22" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="G22" s="44" t="s">
+      <c r="F24" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H22" s="45" t="s">
-        <v>110</v>
-      </c>
-      <c r="I22" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="J22" s="9"/>
-      <c r="K22" s="24"/>
-    </row>
-    <row r="23" spans="1:14" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="41" t="s">
-        <v>107</v>
-      </c>
-      <c r="D23" s="26" t="s">
-        <v>105</v>
-      </c>
-      <c r="E23" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="F23" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="G23" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="H23" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="I23" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="J23" s="9"/>
-      <c r="K23" s="24"/>
-      <c r="M23" s="33"/>
-    </row>
-    <row r="24" spans="1:14" s="33" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="41" t="s">
-        <v>108</v>
-      </c>
-      <c r="D24" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="E24" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="F24" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="G24" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="H24" s="18" t="s">
+      <c r="H24" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="I24" s="17" t="s">
-        <v>90</v>
+      <c r="I24" s="16" t="s">
+        <v>89</v>
       </c>
       <c r="J24" s="9"/>
-      <c r="K24" s="24"/>
+      <c r="K24" s="20"/>
     </row>
     <row r="25" spans="1:14" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D25" s="1"/>
@@ -2560,338 +2541,338 @@
       <c r="J25" s="1"/>
     </row>
     <row r="26" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="24" t="s">
         <v>2</v>
       </c>
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:14" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="47" t="s">
+      <c r="B27" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="39"/>
+      <c r="I27" s="39"/>
+      <c r="J27" s="39"/>
+      <c r="K27" s="39"/>
+    </row>
+    <row r="28" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="C27" s="47"/>
-      <c r="D27" s="47"/>
-      <c r="E27" s="47"/>
-      <c r="F27" s="47"/>
-      <c r="G27" s="47"/>
-      <c r="H27" s="47"/>
-      <c r="I27" s="47"/>
-      <c r="J27" s="47"/>
-      <c r="K27" s="47"/>
-    </row>
-    <row r="28" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="B28" s="47" t="s">
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="39"/>
+      <c r="K28" s="39"/>
+    </row>
+    <row r="29" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="39"/>
+    </row>
+    <row r="30" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="39"/>
+      <c r="K30" s="39"/>
+    </row>
+    <row r="31" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" s="39"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="39"/>
+      <c r="J31" s="39"/>
+      <c r="K31" s="39"/>
+    </row>
+    <row r="32" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="39"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="39"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="39"/>
+      <c r="I32" s="39"/>
+      <c r="J32" s="39"/>
+      <c r="K32" s="39"/>
+      <c r="N32" s="6"/>
+    </row>
+    <row r="33" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" s="39"/>
+      <c r="D33" s="39"/>
+      <c r="E33" s="39"/>
+      <c r="F33" s="39"/>
+      <c r="G33" s="39"/>
+      <c r="H33" s="39"/>
+      <c r="I33" s="39"/>
+      <c r="J33" s="39"/>
+      <c r="K33" s="39"/>
+    </row>
+    <row r="34" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" s="39"/>
+      <c r="D34" s="39"/>
+      <c r="E34" s="39"/>
+      <c r="F34" s="39"/>
+      <c r="G34" s="39"/>
+      <c r="H34" s="39"/>
+      <c r="I34" s="39"/>
+      <c r="J34" s="39"/>
+      <c r="K34" s="39"/>
+    </row>
+    <row r="35" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35" s="39"/>
+      <c r="D35" s="39"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="39"/>
+      <c r="H35" s="39"/>
+      <c r="I35" s="39"/>
+      <c r="J35" s="39"/>
+      <c r="K35" s="39"/>
+      <c r="N35" s="6"/>
+    </row>
+    <row r="36" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="C36" s="39"/>
+      <c r="D36" s="39"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
+      <c r="G36" s="39"/>
+      <c r="H36" s="39"/>
+      <c r="I36" s="39"/>
+      <c r="J36" s="39"/>
+      <c r="K36" s="39"/>
+    </row>
+    <row r="37" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="C37" s="39"/>
+      <c r="D37" s="39"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
+      <c r="G37" s="39"/>
+      <c r="H37" s="39"/>
+      <c r="I37" s="39"/>
+      <c r="J37" s="39"/>
+      <c r="K37" s="39"/>
+    </row>
+    <row r="38" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C38" s="39"/>
+      <c r="D38" s="39"/>
+      <c r="E38" s="39"/>
+      <c r="F38" s="39"/>
+      <c r="G38" s="39"/>
+      <c r="H38" s="39"/>
+      <c r="I38" s="39"/>
+      <c r="J38" s="39"/>
+      <c r="K38" s="39"/>
+    </row>
+    <row r="39" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B39" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="C39" s="39"/>
+      <c r="D39" s="39"/>
+      <c r="E39" s="39"/>
+      <c r="F39" s="39"/>
+      <c r="G39" s="39"/>
+      <c r="H39" s="39"/>
+      <c r="I39" s="39"/>
+      <c r="J39" s="39"/>
+      <c r="K39" s="39"/>
+    </row>
+    <row r="40" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="B40" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="C28" s="47"/>
-      <c r="D28" s="47"/>
-      <c r="E28" s="47"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="47"/>
-      <c r="H28" s="47"/>
-      <c r="I28" s="47"/>
-      <c r="J28" s="47"/>
-      <c r="K28" s="47"/>
-    </row>
-    <row r="29" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="B29" s="47" t="s">
-        <v>92</v>
-      </c>
-      <c r="C29" s="47"/>
-      <c r="D29" s="47"/>
-      <c r="E29" s="47"/>
-      <c r="F29" s="47"/>
-      <c r="G29" s="47"/>
-      <c r="H29" s="47"/>
-      <c r="I29" s="47"/>
-      <c r="J29" s="47"/>
-      <c r="K29" s="47"/>
-    </row>
-    <row r="30" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="B30" s="47" t="s">
-        <v>93</v>
-      </c>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
-      <c r="K30" s="47"/>
-    </row>
-    <row r="31" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="B31" s="47" t="s">
-        <v>94</v>
-      </c>
-      <c r="C31" s="47"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="47"/>
-      <c r="I31" s="47"/>
-      <c r="J31" s="47"/>
-      <c r="K31" s="47"/>
-    </row>
-    <row r="32" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="B32" s="47" t="s">
-        <v>95</v>
-      </c>
-      <c r="C32" s="47"/>
-      <c r="D32" s="47"/>
-      <c r="E32" s="47"/>
-      <c r="F32" s="47"/>
-      <c r="G32" s="47"/>
-      <c r="H32" s="47"/>
-      <c r="I32" s="47"/>
-      <c r="J32" s="47"/>
-      <c r="K32" s="47"/>
-      <c r="N32" s="6"/>
-    </row>
-    <row r="33" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="B33" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="C33" s="47"/>
-      <c r="D33" s="47"/>
-      <c r="E33" s="47"/>
-      <c r="F33" s="47"/>
-      <c r="G33" s="47"/>
-      <c r="H33" s="47"/>
-      <c r="I33" s="47"/>
-      <c r="J33" s="47"/>
-      <c r="K33" s="47"/>
-    </row>
-    <row r="34" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="B34" s="47" t="s">
-        <v>91</v>
-      </c>
-      <c r="C34" s="47"/>
-      <c r="D34" s="47"/>
-      <c r="E34" s="47"/>
-      <c r="F34" s="47"/>
-      <c r="G34" s="47"/>
-      <c r="H34" s="47"/>
-      <c r="I34" s="47"/>
-      <c r="J34" s="47"/>
-      <c r="K34" s="47"/>
-    </row>
-    <row r="35" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="B35" s="47" t="s">
-        <v>97</v>
-      </c>
-      <c r="C35" s="47"/>
-      <c r="D35" s="47"/>
-      <c r="E35" s="47"/>
-      <c r="F35" s="47"/>
-      <c r="G35" s="47"/>
-      <c r="H35" s="47"/>
-      <c r="I35" s="47"/>
-      <c r="J35" s="47"/>
-      <c r="K35" s="47"/>
-      <c r="N35" s="6"/>
-    </row>
-    <row r="36" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="B36" s="47" t="s">
-        <v>98</v>
-      </c>
-      <c r="C36" s="47"/>
-      <c r="D36" s="47"/>
-      <c r="E36" s="47"/>
-      <c r="F36" s="47"/>
-      <c r="G36" s="47"/>
-      <c r="H36" s="47"/>
-      <c r="I36" s="47"/>
-      <c r="J36" s="47"/>
-      <c r="K36" s="47"/>
-    </row>
-    <row r="37" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="38" t="s">
-        <v>24</v>
-      </c>
-      <c r="B37" s="47" t="s">
-        <v>99</v>
-      </c>
-      <c r="C37" s="47"/>
-      <c r="D37" s="47"/>
-      <c r="E37" s="47"/>
-      <c r="F37" s="47"/>
-      <c r="G37" s="47"/>
-      <c r="H37" s="47"/>
-      <c r="I37" s="47"/>
-      <c r="J37" s="47"/>
-      <c r="K37" s="47"/>
-    </row>
-    <row r="38" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="B38" s="47" t="s">
-        <v>100</v>
-      </c>
-      <c r="C38" s="47"/>
-      <c r="D38" s="47"/>
-      <c r="E38" s="47"/>
-      <c r="F38" s="47"/>
-      <c r="G38" s="47"/>
-      <c r="H38" s="47"/>
-      <c r="I38" s="47"/>
-      <c r="J38" s="47"/>
-      <c r="K38" s="47"/>
-    </row>
-    <row r="39" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="B39" s="47" t="s">
+      <c r="C40" s="39"/>
+      <c r="D40" s="39"/>
+      <c r="E40" s="39"/>
+      <c r="F40" s="39"/>
+      <c r="G40" s="39"/>
+      <c r="H40" s="39"/>
+      <c r="I40" s="39"/>
+      <c r="J40" s="39"/>
+      <c r="K40" s="39"/>
+    </row>
+    <row r="41" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="B41" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="C39" s="47"/>
-      <c r="D39" s="47"/>
-      <c r="E39" s="47"/>
-      <c r="F39" s="47"/>
-      <c r="G39" s="47"/>
-      <c r="H39" s="47"/>
-      <c r="I39" s="47"/>
-      <c r="J39" s="47"/>
-      <c r="K39" s="47"/>
-    </row>
-    <row r="40" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="B40" s="47" t="s">
-        <v>89</v>
-      </c>
-      <c r="C40" s="47"/>
-      <c r="D40" s="47"/>
-      <c r="E40" s="47"/>
-      <c r="F40" s="47"/>
-      <c r="G40" s="47"/>
-      <c r="H40" s="47"/>
-      <c r="I40" s="47"/>
-      <c r="J40" s="47"/>
-      <c r="K40" s="47"/>
-    </row>
-    <row r="41" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="B41" s="47" t="s">
+      <c r="C41" s="39"/>
+      <c r="D41" s="39"/>
+      <c r="E41" s="39"/>
+      <c r="F41" s="39"/>
+      <c r="G41" s="39"/>
+      <c r="H41" s="39"/>
+      <c r="I41" s="39"/>
+      <c r="J41" s="39"/>
+      <c r="K41" s="39"/>
+    </row>
+    <row r="42" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="C41" s="47"/>
-      <c r="D41" s="47"/>
-      <c r="E41" s="47"/>
-      <c r="F41" s="47"/>
-      <c r="G41" s="47"/>
-      <c r="H41" s="47"/>
-      <c r="I41" s="47"/>
-      <c r="J41" s="47"/>
-      <c r="K41" s="47"/>
-    </row>
-    <row r="42" spans="1:14" s="33" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="38" t="s">
-        <v>85</v>
-      </c>
-      <c r="B42" s="49" t="s">
-        <v>103</v>
-      </c>
-      <c r="C42" s="49"/>
-      <c r="D42" s="49"/>
-      <c r="E42" s="49"/>
-      <c r="F42" s="49"/>
-      <c r="G42" s="49"/>
-      <c r="H42" s="49"/>
-      <c r="I42" s="49"/>
-      <c r="J42" s="49"/>
-      <c r="K42" s="49"/>
-    </row>
-    <row r="43" spans="1:14" s="33" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="38" t="s">
+      <c r="C42" s="41"/>
+      <c r="D42" s="41"/>
+      <c r="E42" s="41"/>
+      <c r="F42" s="41"/>
+      <c r="G42" s="41"/>
+      <c r="H42" s="41"/>
+      <c r="I42" s="41"/>
+      <c r="J42" s="41"/>
+      <c r="K42" s="41"/>
+    </row>
+    <row r="43" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="B43" s="49" t="s">
-        <v>112</v>
-      </c>
-      <c r="C43" s="49"/>
-      <c r="D43" s="49"/>
-      <c r="E43" s="49"/>
-      <c r="F43" s="49"/>
-      <c r="G43" s="49"/>
-      <c r="H43" s="49"/>
-      <c r="I43" s="49"/>
-      <c r="J43" s="49"/>
-      <c r="K43" s="49"/>
+      <c r="B43" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="C43" s="41"/>
+      <c r="D43" s="41"/>
+      <c r="E43" s="41"/>
+      <c r="F43" s="41"/>
+      <c r="G43" s="41"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
+      <c r="K43" s="41"/>
     </row>
     <row r="44" spans="1:14" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="48"/>
-      <c r="C44" s="48"/>
-      <c r="D44" s="48"/>
-      <c r="E44" s="48"/>
-      <c r="F44" s="48"/>
-      <c r="G44" s="48"/>
-      <c r="H44" s="48"/>
-      <c r="I44" s="48"/>
-      <c r="J44" s="48"/>
-      <c r="K44" s="48"/>
+      <c r="B44" s="40"/>
+      <c r="C44" s="40"/>
+      <c r="D44" s="40"/>
+      <c r="E44" s="40"/>
+      <c r="F44" s="40"/>
+      <c r="G44" s="40"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
+      <c r="K44" s="40"/>
     </row>
     <row r="45" spans="1:14" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="30" t="s">
+      <c r="B45" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="D45" s="29" t="s">
+      <c r="D45" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="E45" s="13" t="s">
+      <c r="E45" s="12" t="s">
         <v>77</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G45" s="17" t="s">
+      <c r="G45" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="H45" s="18" t="s">
+      <c r="H45" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="I45" s="17" t="s">
+      <c r="I45" s="16" t="s">
         <v>74</v>
       </c>
       <c r="J45" s="9"/>
-      <c r="K45" s="31"/>
+      <c r="K45" s="26"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B46" s="32" t="s">
+      <c r="B46" s="27" t="s">
         <v>44</v>
       </c>
       <c r="D46">
@@ -2915,6 +2896,15 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B36:K36"/>
+    <mergeCell ref="B44:K44"/>
+    <mergeCell ref="B42:K42"/>
+    <mergeCell ref="B43:K43"/>
+    <mergeCell ref="B40:K40"/>
+    <mergeCell ref="B41:K41"/>
+    <mergeCell ref="B37:K37"/>
+    <mergeCell ref="B38:K38"/>
+    <mergeCell ref="B39:K39"/>
     <mergeCell ref="B32:K32"/>
     <mergeCell ref="B33:K33"/>
     <mergeCell ref="B34:K34"/>
@@ -2924,19 +2914,10 @@
     <mergeCell ref="B29:K29"/>
     <mergeCell ref="B30:K30"/>
     <mergeCell ref="B31:K31"/>
-    <mergeCell ref="B36:K36"/>
-    <mergeCell ref="B44:K44"/>
-    <mergeCell ref="B42:K42"/>
-    <mergeCell ref="B43:K43"/>
-    <mergeCell ref="B40:K40"/>
-    <mergeCell ref="B41:K41"/>
-    <mergeCell ref="B37:K37"/>
-    <mergeCell ref="B38:K38"/>
-    <mergeCell ref="B39:K39"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="53" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="60" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>